<commit_message>
Published state of ETDataset for deploy March 2024
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/buildings/buildings_space_heater_heatpump_surface_water_water_ts_electricity.xlsx
+++ b/nodes_source_analyses/energy/buildings/buildings_space_heater_heatpump_surface_water_water_ts_electricity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10211"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koenvanbemmelen/work/etdataset/nodes_source_analyses/energy/buildings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/nodes_source_analyses/energy/buildings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1868453-672B-DD41-983D-12A8215726EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C44FC4C-FC9D-0C46-858C-68C589E18C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="156">
   <si>
     <t>Source</t>
   </si>
@@ -417,15 +417,9 @@
     <t>input.electricity</t>
   </si>
   <si>
-    <t>Koen van Bemmelen</t>
-  </si>
-  <si>
     <t>Quintel</t>
   </si>
   <si>
-    <t>buildings_space_heater_heatpump_surface_water_water_ts_electricity.converter.ad</t>
-  </si>
-  <si>
     <t>Weighted average cost of capital</t>
   </si>
   <si>
@@ -616,6 +610,15 @@
   </si>
   <si>
     <t>eur/unit/year</t>
+  </si>
+  <si>
+    <t>Mathijs Bijkerk</t>
+  </si>
+  <si>
+    <t>buildings_space_heater_heatpump_surface_water_water_ts_electricity.ad</t>
+  </si>
+  <si>
+    <t>Quintel assumption to scale to 11 kW instead of 4.4 MW</t>
   </si>
 </sst>
 </file>
@@ -916,7 +919,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1147,21 +1150,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="256">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1424,21 +1412,16 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="161">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1516,23 +1499,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1684,6 +1652,28 @@
     <xf numFmtId="0" fontId="26" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="256">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2881,181 +2871,201 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="20" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="55.1640625" style="13" customWidth="1"/>
-    <col min="4" max="16384" width="10.6640625" style="13"/>
+    <col min="1" max="1" width="3.5" style="17" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="55.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" style="10" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="18" customFormat="1">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-    </row>
-    <row r="2" spans="1:3" ht="21">
+    <row r="1" spans="1:4" s="15" customFormat="1">
+      <c r="A1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" ht="21">
       <c r="A2" s="1"/>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="19"/>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1"/>
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" s="155"/>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1"/>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="143" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="156"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="157" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="73"/>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1"/>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="75"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" s="158"/>
+      <c r="D9" s="155"/>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1"/>
-      <c r="B10" s="57"/>
-      <c r="C10" s="76"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="54"/>
+      <c r="C10" s="144"/>
+      <c r="D10" s="156"/>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1"/>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="77" t="s">
+      <c r="C11" s="145" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" thickBot="1">
+      <c r="D11" s="156"/>
+    </row>
+    <row r="12" spans="1:4" ht="17" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="78" t="s">
+      <c r="B12" s="54"/>
+      <c r="C12" s="146" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" thickBot="1">
+      <c r="D12" s="156"/>
+    </row>
+    <row r="13" spans="1:4" ht="17" thickBot="1">
       <c r="A13" s="1"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="79" t="s">
+      <c r="B13" s="54"/>
+      <c r="C13" s="160" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="156"/>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="76" t="s">
+      <c r="B14" s="54"/>
+      <c r="C14" s="144" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" s="156"/>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="76"/>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="B15" s="54"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="156"/>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="80" t="s">
+      <c r="C16" s="147" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" s="156"/>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
-      <c r="B17" s="57"/>
-      <c r="C17" s="81" t="s">
+      <c r="B17" s="54"/>
+      <c r="C17" s="148" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" s="156"/>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="82" t="s">
+      <c r="B18" s="54"/>
+      <c r="C18" s="149" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" s="156"/>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1"/>
-      <c r="B19" s="57"/>
-      <c r="C19" s="83" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="150" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" s="156"/>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
-      <c r="B20" s="58"/>
-      <c r="C20" s="84" t="s">
+      <c r="B20" s="55"/>
+      <c r="C20" s="151" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" s="156"/>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
-      <c r="B21" s="58"/>
-      <c r="C21" s="85" t="s">
+      <c r="B21" s="55"/>
+      <c r="C21" s="152" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" s="156"/>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="86" t="s">
+      <c r="B22" s="55"/>
+      <c r="C22" s="153" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="B23" s="58"/>
-      <c r="C23" s="87" t="s">
+      <c r="D22" s="156"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="B23" s="55"/>
+      <c r="C23" s="154" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="B24" s="88"/>
-      <c r="C24" s="89"/>
+      <c r="D23" s="156"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="B24" s="72"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="73"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3068,538 +3078,528 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:J34"/>
+  <dimension ref="B2:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="46" style="24" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="24" customWidth="1"/>
-    <col min="6" max="6" width="4.5" style="24" customWidth="1"/>
-    <col min="7" max="7" width="45" style="24" customWidth="1"/>
-    <col min="8" max="8" width="5.1640625" style="24" customWidth="1"/>
-    <col min="9" max="9" width="46.1640625" style="24" customWidth="1"/>
-    <col min="10" max="10" width="5.5" style="24" customWidth="1"/>
-    <col min="11" max="16384" width="10.6640625" style="24"/>
+    <col min="1" max="1" width="3.33203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="3.6640625" style="21" customWidth="1"/>
+    <col min="3" max="3" width="62.1640625" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="21" customWidth="1"/>
+    <col min="6" max="6" width="4.5" style="21" customWidth="1"/>
+    <col min="7" max="7" width="45" style="21" customWidth="1"/>
+    <col min="8" max="8" width="5.1640625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="46.1640625" style="21" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="21" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="21"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="154"/>
+      <c r="C2" s="135"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="136"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="155"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="157"/>
+      <c r="B3" s="137"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="139"/>
     </row>
     <row r="4" spans="2:10" ht="31" customHeight="1">
-      <c r="B4" s="158"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="160"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="141"/>
+      <c r="D4" s="141"/>
+      <c r="E4" s="142"/>
     </row>
     <row r="5" spans="2:10" ht="17" thickBot="1"/>
     <row r="6" spans="2:10">
-      <c r="B6" s="26"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="27"/>
-    </row>
-    <row r="7" spans="2:10" s="32" customFormat="1" ht="19">
-      <c r="B7" s="59"/>
-      <c r="C7" s="10" t="s">
+      <c r="B6" s="23"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" s="29" customFormat="1" ht="19">
+      <c r="B7" s="56"/>
+      <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="65"/>
-    </row>
-    <row r="8" spans="2:10" s="32" customFormat="1" ht="19">
-      <c r="B8" s="15"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="33"/>
-    </row>
-    <row r="9" spans="2:10" s="32" customFormat="1" ht="20" thickBot="1">
-      <c r="B9" s="15"/>
-      <c r="C9" s="9" t="s">
+      <c r="J7" s="62"/>
+    </row>
+    <row r="8" spans="2:10" s="29" customFormat="1" ht="19">
+      <c r="B8" s="12"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="30"/>
+    </row>
+    <row r="9" spans="2:10" s="29" customFormat="1" ht="20" thickBot="1">
+      <c r="B9" s="12"/>
+      <c r="C9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="33"/>
-    </row>
-    <row r="10" spans="2:10" s="32" customFormat="1" ht="20" thickBot="1">
-      <c r="B10" s="15"/>
-      <c r="C10" s="70" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="30"/>
+    </row>
+    <row r="10" spans="2:10" s="29" customFormat="1" ht="20" thickBot="1">
+      <c r="B10" s="12"/>
+      <c r="C10" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="146">
+      <c r="E10" s="128">
         <f>ROUND('Research data'!E6,3)</f>
         <v>0.69699999999999995</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="2:10" s="32" customFormat="1" ht="20" thickBot="1">
-      <c r="B11" s="15"/>
-      <c r="C11" s="72" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="30"/>
+    </row>
+    <row r="11" spans="2:10" s="29" customFormat="1" ht="20" thickBot="1">
+      <c r="B11" s="12"/>
+      <c r="C11" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="146">
+      <c r="E11" s="128">
         <f>ROUND('Research data'!E7,3)</f>
         <v>0.30299999999999999</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="33"/>
-    </row>
-    <row r="12" spans="2:10" s="32" customFormat="1" ht="20" thickBot="1">
-      <c r="B12" s="15"/>
-      <c r="C12" s="92" t="s">
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="30"/>
+    </row>
+    <row r="12" spans="2:10" s="29" customFormat="1" ht="20" thickBot="1">
+      <c r="B12" s="12"/>
+      <c r="C12" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="34">
+      <c r="E12" s="31">
         <v>1</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="33"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="30"/>
     </row>
     <row r="13" spans="2:10" ht="17" thickBot="1">
-      <c r="B13" s="28"/>
-      <c r="C13" s="90" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="161" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="31">
         <v>0</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="122" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="66"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="2:10" ht="17" thickBot="1">
-      <c r="B14" s="28"/>
-      <c r="C14" s="91" t="s">
+      <c r="B14" s="25"/>
+      <c r="C14" s="162" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="35">
+      <c r="E14" s="32">
         <f>'Research data'!E9</f>
         <v>1750</v>
       </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="122" t="s">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="63"/>
+    </row>
+    <row r="15" spans="2:10" ht="17" thickBot="1">
+      <c r="B15" s="25"/>
+      <c r="C15" s="161" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="22"/>
+      <c r="I15" s="121" t="s">
+        <v>140</v>
+      </c>
+      <c r="J15" s="63"/>
+    </row>
+    <row r="16" spans="2:10" ht="17" thickBot="1">
+      <c r="B16" s="25"/>
+      <c r="C16" s="161" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="31">
+        <f>'Research data'!E8</f>
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="63"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="25"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
+      <c r="G17" s="45"/>
+      <c r="J17" s="63"/>
+    </row>
+    <row r="18" spans="2:10" ht="17" thickBot="1">
+      <c r="B18" s="25"/>
+      <c r="C18" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59"/>
+      <c r="G18" s="45"/>
+      <c r="J18" s="63"/>
+    </row>
+    <row r="19" spans="2:10" ht="17" thickBot="1">
+      <c r="B19" s="25"/>
+      <c r="C19" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="132">
+        <f>'Research data'!E17</f>
+        <v>11861</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="22"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="63"/>
+    </row>
+    <row r="20" spans="2:10" ht="17" thickBot="1">
+      <c r="B20" s="25"/>
+      <c r="C20" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="32">
+        <v>0</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="H20" s="22"/>
+      <c r="I20" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="J14" s="66"/>
-    </row>
-    <row r="15" spans="2:10" ht="17" thickBot="1">
-      <c r="B15" s="28"/>
-      <c r="C15" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E15" s="35">
+      <c r="J20" s="63"/>
+    </row>
+    <row r="21" spans="2:10" ht="17" thickBot="1">
+      <c r="B21" s="25"/>
+      <c r="C21" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="32">
         <v>0</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="139" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" s="66"/>
-    </row>
-    <row r="16" spans="2:10" ht="17" thickBot="1">
-      <c r="B16" s="28"/>
-      <c r="C16" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" s="34">
-        <f>'Research data'!E8</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="66"/>
-    </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="28"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="J17" s="66"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="28"/>
-      <c r="C18" s="48"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
-      <c r="G18" s="48"/>
-      <c r="J18" s="66"/>
-    </row>
-    <row r="19" spans="2:10" ht="17" thickBot="1">
-      <c r="B19" s="28"/>
-      <c r="C19" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D19" s="61"/>
-      <c r="E19" s="62"/>
-      <c r="G19" s="48"/>
-      <c r="J19" s="66"/>
-    </row>
-    <row r="20" spans="2:10" ht="17" thickBot="1">
-      <c r="B20" s="28"/>
-      <c r="C20" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="F21" s="22"/>
+      <c r="G21" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="J21" s="63"/>
+    </row>
+    <row r="22" spans="2:10" ht="17" thickBot="1">
+      <c r="B22" s="25"/>
+      <c r="C22" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="150">
-        <f>'Research data'!E17</f>
-        <v>4744522</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="66"/>
-    </row>
-    <row r="21" spans="2:10" ht="17" thickBot="1">
-      <c r="B21" s="28"/>
-      <c r="C21" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="35">
+      <c r="E22" s="32">
         <v>0</v>
       </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="J21" s="66"/>
-    </row>
-    <row r="22" spans="2:10" ht="17" thickBot="1">
-      <c r="B22" s="28"/>
-      <c r="C22" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" s="35">
+      <c r="F22" s="22"/>
+      <c r="G22" s="118" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="J22" s="63"/>
+    </row>
+    <row r="23" spans="2:10" ht="17" thickBot="1">
+      <c r="B23" s="25"/>
+      <c r="C23" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="131">
+        <f>'Research data'!E18</f>
+        <v>277</v>
+      </c>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="22"/>
+      <c r="I23" s="52"/>
+      <c r="J23" s="63"/>
+    </row>
+    <row r="24" spans="2:10" ht="17" thickBot="1">
+      <c r="B24" s="25"/>
+      <c r="C24" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E24" s="31">
         <v>0</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="139" t="s">
+      <c r="F24" s="22"/>
+      <c r="G24" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H24" s="22"/>
+      <c r="I24" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="63"/>
+    </row>
+    <row r="25" spans="2:10" ht="17" thickBot="1">
+      <c r="B25" s="25"/>
+      <c r="C25" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="60">
+        <v>0</v>
+      </c>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="22"/>
+      <c r="I25" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="J22" s="66"/>
-    </row>
-    <row r="23" spans="2:10" ht="17" thickBot="1">
-      <c r="B23" s="28"/>
-      <c r="C23" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E23" s="35">
+      <c r="J25" s="63"/>
+    </row>
+    <row r="26" spans="2:10" ht="17" thickBot="1">
+      <c r="B26" s="25"/>
+      <c r="C26" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="31">
+        <v>0.04</v>
+      </c>
+      <c r="F26" s="22"/>
+      <c r="G26" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="H26" s="22"/>
+      <c r="I26" s="104" t="s">
+        <v>91</v>
+      </c>
+      <c r="J26" s="63"/>
+    </row>
+    <row r="27" spans="2:10" ht="17" thickBot="1">
+      <c r="B27" s="25"/>
+      <c r="C27" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="32">
         <v>0</v>
       </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="136" t="s">
-        <v>130</v>
-      </c>
-      <c r="H23" s="25"/>
-      <c r="I23" s="139" t="s">
-        <v>92</v>
-      </c>
-      <c r="J23" s="66"/>
-    </row>
-    <row r="24" spans="2:10" ht="17" thickBot="1">
-      <c r="B24" s="28"/>
-      <c r="C24" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E24" s="149">
-        <f>'Research data'!E18</f>
-        <v>110639</v>
-      </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="25"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="66"/>
-    </row>
-    <row r="25" spans="2:10" ht="17" thickBot="1">
-      <c r="B25" s="28"/>
-      <c r="C25" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" s="34">
-        <v>0</v>
-      </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="139" t="s">
-        <v>92</v>
-      </c>
-      <c r="J25" s="66"/>
-    </row>
-    <row r="26" spans="2:10" ht="17" thickBot="1">
-      <c r="B26" s="28"/>
-      <c r="C26" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E26" s="63">
-        <v>0</v>
-      </c>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="123" t="s">
-        <v>94</v>
-      </c>
-      <c r="J26" s="66"/>
-    </row>
-    <row r="27" spans="2:10" ht="17" thickBot="1">
-      <c r="B27" s="28"/>
-      <c r="C27" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E27" s="34">
-        <v>0.04</v>
-      </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="92" t="s">
-        <v>91</v>
-      </c>
-      <c r="H27" s="25"/>
-      <c r="I27" s="122" t="s">
-        <v>93</v>
-      </c>
-      <c r="J27" s="66"/>
-    </row>
-    <row r="28" spans="2:10" ht="17" thickBot="1">
-      <c r="B28" s="28"/>
-      <c r="C28" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E28" s="35">
-        <v>0</v>
-      </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="122" t="s">
-        <v>92</v>
-      </c>
-      <c r="J28" s="66"/>
-    </row>
-    <row r="29" spans="2:10">
-      <c r="B29" s="28"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="J29" s="66"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="J27" s="63"/>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28" s="25"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="J28" s="63"/>
+    </row>
+    <row r="29" spans="2:10" ht="17" thickBot="1">
+      <c r="B29" s="25"/>
+      <c r="C29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="58"/>
+      <c r="E29" s="61"/>
+      <c r="J29" s="63"/>
     </row>
     <row r="30" spans="2:10" ht="17" thickBot="1">
-      <c r="B30" s="28"/>
-      <c r="C30" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="61"/>
-      <c r="E30" s="64"/>
-      <c r="J30" s="66"/>
-    </row>
-    <row r="31" spans="2:10" ht="17" thickBot="1">
-      <c r="B31" s="28"/>
-      <c r="C31" s="71" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D30" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="35">
+      <c r="E30" s="32">
         <f>'Research data'!E13</f>
         <v>0</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25" t="s">
+      <c r="F30" s="22"/>
+      <c r="G30" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="66"/>
-    </row>
-    <row r="32" spans="2:10" ht="17" thickBot="1">
-      <c r="B32" s="28"/>
-      <c r="C32" s="25" t="s">
+      <c r="H30" s="22"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="63"/>
+    </row>
+    <row r="31" spans="2:10" ht="17" thickBot="1">
+      <c r="B31" s="25"/>
+      <c r="C31" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D31" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="150">
+      <c r="E31" s="132">
         <f>'Research data'!E14</f>
         <v>30</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25" t="s">
+      <c r="F31" s="22"/>
+      <c r="G31" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="25"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="66"/>
-    </row>
-    <row r="33" spans="2:10" ht="17" thickBot="1">
-      <c r="B33" s="28"/>
-      <c r="C33" s="25" t="s">
+      <c r="H31" s="22"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="63"/>
+    </row>
+    <row r="32" spans="2:10" ht="17" thickBot="1">
+      <c r="B32" s="25"/>
+      <c r="C32" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D32" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="35">
+      <c r="E32" s="32">
         <v>0</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="122" t="s">
-        <v>92</v>
-      </c>
-      <c r="J33" s="66"/>
-    </row>
-    <row r="34" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="31"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="104" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="63"/>
+    </row>
+    <row r="33" spans="2:10" ht="20" customHeight="1" thickBot="1">
+      <c r="B33" s="26"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3618,424 +3618,429 @@
   <dimension ref="B1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="3.5" style="48" customWidth="1"/>
-    <col min="3" max="3" width="42.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="48" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" style="48" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" style="48" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="49" customWidth="1"/>
-    <col min="9" max="9" width="15.83203125" style="48" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" style="48"/>
-    <col min="11" max="11" width="59.5" style="48" customWidth="1"/>
-    <col min="12" max="16384" width="10.6640625" style="48"/>
+    <col min="1" max="2" width="3.5" style="45" customWidth="1"/>
+    <col min="3" max="3" width="42.1640625" style="45" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="45" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" style="45" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" style="45" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="45" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="46" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="45" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="45"/>
+    <col min="11" max="11" width="59.5" style="45" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="45"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="50"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="93"/>
-    </row>
-    <row r="3" spans="2:11" s="9" customFormat="1">
-      <c r="B3" s="15"/>
-      <c r="C3" s="67" t="s">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="75"/>
+    </row>
+    <row r="3" spans="2:11" s="6" customFormat="1">
+      <c r="B3" s="12"/>
+      <c r="C3" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="D3" s="67" t="s">
+      <c r="D3" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67" t="s">
-        <v>138</v>
-      </c>
-      <c r="H3" s="67" t="s">
-        <v>139</v>
-      </c>
-      <c r="I3" s="67" t="s">
+      <c r="F3" s="64"/>
+      <c r="G3" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="H3" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="47"/>
-      <c r="K3" s="94" t="s">
+      <c r="J3" s="44"/>
+      <c r="K3" s="76" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="53"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
-      <c r="G4" s="96"/>
-      <c r="H4" s="96"/>
-      <c r="I4" s="96"/>
-      <c r="J4" s="97"/>
-      <c r="K4" s="98"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="80"/>
     </row>
     <row r="5" spans="2:11" ht="17" thickBot="1">
-      <c r="B5" s="53"/>
-      <c r="C5" s="99" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="99"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="130"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="82"/>
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="112"/>
     </row>
     <row r="6" spans="2:11" ht="17" thickBot="1">
-      <c r="B6" s="53"/>
-      <c r="C6" s="101" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="83" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="99"/>
-      <c r="E6" s="73">
+      <c r="D6" s="81"/>
+      <c r="E6" s="70">
         <f>H6</f>
         <v>0.69696969696969702</v>
       </c>
-      <c r="F6" s="100"/>
-      <c r="G6" s="73">
+      <c r="F6" s="82"/>
+      <c r="G6" s="70">
         <f>1-G7</f>
         <v>0.78260869565217384</v>
       </c>
-      <c r="H6" s="73">
+      <c r="H6" s="70">
         <f>1-H7</f>
         <v>0.69696969696969702</v>
       </c>
-      <c r="I6" s="104"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="130" t="s">
-        <v>152</v>
+      <c r="I6" s="86"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="112" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="17" thickBot="1">
-      <c r="B7" s="53"/>
-      <c r="C7" s="101" t="s">
+      <c r="B7" s="50"/>
+      <c r="C7" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="99"/>
-      <c r="E7" s="73">
+      <c r="D7" s="81"/>
+      <c r="E7" s="70">
         <f>H7</f>
         <v>0.30303030303030304</v>
       </c>
-      <c r="F7" s="100"/>
-      <c r="G7" s="73">
+      <c r="F7" s="82"/>
+      <c r="G7" s="70">
         <f>1/Notes!$H$10</f>
         <v>0.21739130434782611</v>
       </c>
-      <c r="H7" s="73">
+      <c r="H7" s="70">
         <f>1/Notes!$H$9</f>
         <v>0.30303030303030304</v>
       </c>
-      <c r="I7" s="104"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="130" t="s">
-        <v>152</v>
+      <c r="I7" s="86"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="112" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="17" thickBot="1">
-      <c r="B8" s="53"/>
-      <c r="C8" s="102" t="s">
+      <c r="B8" s="50"/>
+      <c r="C8" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="103" t="s">
+      <c r="D8" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="141">
-        <f>G8</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F8" s="104"/>
-      <c r="G8" s="141">
+      <c r="E8" s="70">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F8" s="86"/>
+      <c r="G8" s="123">
         <f>ROUND(Notes!$H$8,1)</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="130"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="112" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="9" spans="2:11" ht="17" thickBot="1">
-      <c r="B9" s="53"/>
-      <c r="C9" s="147" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="148" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="141">
+      <c r="B9" s="50"/>
+      <c r="C9" s="129" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="130" t="s">
+        <v>139</v>
+      </c>
+      <c r="E9" s="123">
         <f>G9</f>
         <v>1750</v>
       </c>
-      <c r="F9" s="104"/>
-      <c r="G9" s="141">
+      <c r="F9" s="86"/>
+      <c r="G9" s="123">
         <f>Notes!H6</f>
         <v>1750</v>
       </c>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="130"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="112"/>
     </row>
     <row r="10" spans="2:11">
-      <c r="B10" s="53"/>
-      <c r="C10" s="105"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="106"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="130"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="87"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="112"/>
     </row>
     <row r="11" spans="2:11" ht="17" thickBot="1">
-      <c r="B11" s="53"/>
-      <c r="C11" s="99" t="s">
+      <c r="B11" s="50"/>
+      <c r="C11" s="81" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="99"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="107"/>
-      <c r="G11" s="107"/>
-      <c r="H11" s="107"/>
-      <c r="I11" s="107"/>
-      <c r="J11" s="108"/>
-      <c r="K11" s="143"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="125"/>
     </row>
     <row r="12" spans="2:11" ht="17" thickBot="1">
-      <c r="B12" s="53"/>
-      <c r="C12" s="109" t="s">
+      <c r="B12" s="50"/>
+      <c r="C12" s="91" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="110" t="s">
+      <c r="D12" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="69">
+      <c r="E12" s="66">
         <f>ROUND(0,0)</f>
         <v>0</v>
       </c>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="107"/>
-      <c r="I12" s="107"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="143" t="s">
-        <v>92</v>
+      <c r="F12" s="89"/>
+      <c r="G12" s="89"/>
+      <c r="H12" s="89"/>
+      <c r="I12" s="89"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="125" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="2:11" ht="17" thickBot="1">
-      <c r="B13" s="53"/>
-      <c r="C13" s="142" t="s">
-        <v>140</v>
-      </c>
-      <c r="D13" s="103" t="s">
+      <c r="B13" s="50"/>
+      <c r="C13" s="124" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="69">
+      <c r="E13" s="66">
         <f>ROUND(0,0)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="107"/>
-      <c r="I13" s="107"/>
-      <c r="J13" s="108"/>
-      <c r="K13" s="143" t="s">
-        <v>92</v>
+      <c r="F13" s="89"/>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
+      <c r="I13" s="89"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="125" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="2:11" ht="17" thickBot="1">
-      <c r="B14" s="53"/>
-      <c r="C14" s="109" t="s">
+      <c r="B14" s="50"/>
+      <c r="C14" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="E14" s="69">
+      <c r="E14" s="66">
         <f>G14</f>
         <v>30</v>
       </c>
-      <c r="F14" s="106"/>
-      <c r="G14" s="69">
+      <c r="F14" s="88"/>
+      <c r="G14" s="66">
         <f>Notes!H7</f>
         <v>30</v>
       </c>
-      <c r="H14" s="106"/>
-      <c r="I14" s="106"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="130"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="93"/>
+      <c r="K14" s="112"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="53"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="108"/>
-      <c r="H15" s="108"/>
-      <c r="I15" s="108"/>
-      <c r="J15" s="111"/>
-      <c r="K15" s="130"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="93"/>
+      <c r="K15" s="112"/>
     </row>
     <row r="16" spans="2:11" ht="17" thickBot="1">
-      <c r="B16" s="53"/>
-      <c r="C16" s="112" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="112"/>
-      <c r="E16" s="108"/>
-      <c r="F16" s="108"/>
-      <c r="G16" s="108"/>
-      <c r="H16" s="108"/>
-      <c r="I16" s="108"/>
-      <c r="J16" s="108"/>
-      <c r="K16" s="130"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="112"/>
     </row>
     <row r="17" spans="2:11" ht="17" thickBot="1">
-      <c r="B17" s="53"/>
-      <c r="C17" s="113" t="s">
+      <c r="B17" s="50"/>
+      <c r="C17" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="113" t="s">
+      <c r="D17" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="145">
-        <f>ROUND(AVERAGE(G17:I17),0)</f>
-        <v>4744522</v>
-      </c>
-      <c r="F17" s="108"/>
-      <c r="G17" s="144">
+      <c r="E17" s="127">
+        <f>ROUND(AVERAGE(G17:I17)/G8*E8,0)</f>
+        <v>11861</v>
+      </c>
+      <c r="F17" s="90"/>
+      <c r="G17" s="126">
         <f>ROUND(Notes!H12,0)</f>
         <v>7012500</v>
       </c>
-      <c r="H17" s="144">
+      <c r="H17" s="126">
         <f>ROUND(Notes!H13,0)</f>
         <v>5497685</v>
       </c>
-      <c r="I17" s="144">
+      <c r="I17" s="126">
         <f>SUM(Notes!H14:H15)</f>
         <v>1723379.6296296294</v>
       </c>
-      <c r="J17" s="106"/>
-      <c r="K17" s="130"/>
+      <c r="J17" s="88"/>
+      <c r="K17" s="112" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="18" spans="2:11" ht="17" thickBot="1">
-      <c r="B18" s="53"/>
-      <c r="C18" s="114" t="s">
+      <c r="B18" s="50"/>
+      <c r="C18" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="D18" s="115" t="s">
+      <c r="D18" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="145">
-        <f>ROUND(AVERAGE(G18:I18),0)</f>
-        <v>110639</v>
-      </c>
-      <c r="F18" s="108"/>
-      <c r="G18" s="144">
+      <c r="E18" s="127">
+        <f>ROUND(AVERAGE(G18:I18)/G8*E8,0)</f>
+        <v>277</v>
+      </c>
+      <c r="F18" s="90"/>
+      <c r="G18" s="126">
         <f>ROUND(Notes!H17,0)</f>
         <v>137500</v>
       </c>
-      <c r="H18" s="144">
+      <c r="H18" s="126">
         <f>ROUND(Notes!H16,0)</f>
         <v>118750</v>
       </c>
-      <c r="I18" s="144">
+      <c r="I18" s="126">
         <f>SUM(Notes!H18:H19)</f>
         <v>75666.666666666672</v>
       </c>
-      <c r="J18" s="106"/>
-      <c r="K18" s="130"/>
+      <c r="J18" s="88"/>
+      <c r="K18" s="112" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="19" spans="2:11" ht="17" thickBot="1">
-      <c r="B19" s="53"/>
-      <c r="C19" s="113" t="s">
+      <c r="B19" s="50"/>
+      <c r="C19" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="116" t="s">
+      <c r="D19" s="98" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="151">
+      <c r="E19" s="133">
         <f>ROUND(E18/(E8*1000),0)</f>
         <v>25</v>
       </c>
-      <c r="F19" s="108"/>
-      <c r="G19" s="108"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="106"/>
-      <c r="K19" s="130"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="90"/>
+      <c r="I19" s="90"/>
+      <c r="J19" s="88"/>
+      <c r="K19" s="112"/>
     </row>
     <row r="20" spans="2:11" ht="17" thickBot="1">
-      <c r="B20" s="53"/>
-      <c r="C20" s="114" t="s">
+      <c r="B20" s="50"/>
+      <c r="C20" s="96" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="103" t="s">
+      <c r="D20" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="54">
+      <c r="E20" s="51">
         <v>0</v>
       </c>
-      <c r="F20" s="106"/>
-      <c r="G20" s="106"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="106"/>
-      <c r="K20" s="130" t="s">
-        <v>92</v>
+      <c r="F20" s="88"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="112" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="2:11" ht="17" thickBot="1">
-      <c r="B21" s="53"/>
-      <c r="C21" s="113" t="s">
+      <c r="B21" s="50"/>
+      <c r="C21" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="117" t="s">
+      <c r="D21" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="51">
         <v>0</v>
       </c>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="130" t="s">
-        <v>92</v>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="112" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1">
-      <c r="B22" s="118"/>
-      <c r="C22" s="119"/>
-      <c r="D22" s="119"/>
-      <c r="E22" s="119"/>
-      <c r="F22" s="119"/>
-      <c r="G22" s="119"/>
-      <c r="H22" s="119"/>
-      <c r="I22" s="119"/>
-      <c r="J22" s="120"/>
-      <c r="K22" s="121"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="101"/>
+      <c r="E22" s="101"/>
+      <c r="F22" s="101"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="101"/>
+      <c r="I22" s="101"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="103"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4056,284 +4061,284 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="36" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="36" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="36" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" style="36" customWidth="1"/>
-    <col min="5" max="5" width="33" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="36" customWidth="1"/>
-    <col min="7" max="9" width="12.1640625" style="36" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="37" customWidth="1"/>
-    <col min="11" max="11" width="66" style="36" customWidth="1"/>
-    <col min="12" max="16384" width="33.1640625" style="36"/>
+    <col min="1" max="1" width="3.33203125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="33" customWidth="1"/>
+    <col min="3" max="3" width="28.6640625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="33" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="33" customWidth="1"/>
+    <col min="7" max="9" width="12.1640625" style="33" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="34" customWidth="1"/>
+    <col min="11" max="11" width="66" style="33" customWidth="1"/>
+    <col min="12" max="16384" width="33.1640625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17" thickBot="1"/>
     <row r="2" spans="2:11">
-      <c r="B2" s="38"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="126"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="108"/>
     </row>
     <row r="3" spans="2:11">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="127"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="109"/>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="41"/>
-      <c r="K4" s="127"/>
+      <c r="B4" s="38"/>
+      <c r="K4" s="109"/>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45" t="s">
+      <c r="B5" s="41"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="45" t="s">
+      <c r="G5" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="45" t="s">
+      <c r="H5" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="I5" s="45" t="s">
+      <c r="I5" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" s="43" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="110" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" s="38"/>
+      <c r="K6" s="109"/>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" s="38"/>
+      <c r="K7" s="109"/>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" s="38"/>
+      <c r="C8" s="107"/>
+      <c r="D8" s="107"/>
+      <c r="E8" s="107" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" s="107">
+        <v>2021</v>
+      </c>
+      <c r="H8" s="107"/>
+      <c r="I8" s="111">
+        <v>45139</v>
+      </c>
+      <c r="J8" s="113" t="s">
+        <v>108</v>
+      </c>
+      <c r="K8" s="112"/>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" s="38"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="107" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="107">
+        <v>2018</v>
+      </c>
+      <c r="H9" s="107"/>
+      <c r="I9" s="111">
+        <v>45200</v>
+      </c>
+      <c r="J9" s="113" t="s">
         <v>109</v>
       </c>
-      <c r="J5" s="46" t="s">
-        <v>83</v>
-      </c>
-      <c r="K5" s="128" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" s="41"/>
-      <c r="K6" s="127"/>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="41"/>
-      <c r="K7" s="127"/>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" s="41"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125" t="s">
-        <v>101</v>
-      </c>
-      <c r="F8" s="125" t="s">
+      <c r="K9" s="112"/>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" s="38"/>
+      <c r="C10" s="113"/>
+      <c r="D10" s="107"/>
+      <c r="E10" s="107" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="G8" s="125">
-        <v>2021</v>
-      </c>
-      <c r="H8" s="125"/>
-      <c r="I8" s="129">
-        <v>45139</v>
-      </c>
-      <c r="J8" s="131" t="s">
-        <v>110</v>
-      </c>
-      <c r="K8" s="130"/>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" s="41"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="125" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="125">
-        <v>2018</v>
-      </c>
-      <c r="H9" s="125"/>
-      <c r="I9" s="129">
+      <c r="G10" s="107">
+        <v>2019</v>
+      </c>
+      <c r="H10" s="107"/>
+      <c r="I10" s="111">
         <v>45200</v>
       </c>
-      <c r="J9" s="131" t="s">
-        <v>111</v>
-      </c>
-      <c r="K9" s="130"/>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" s="41"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="125" t="s">
-        <v>86</v>
-      </c>
-      <c r="G10" s="125">
-        <v>2019</v>
-      </c>
-      <c r="H10" s="125"/>
-      <c r="I10" s="129">
-        <v>45200</v>
-      </c>
-      <c r="J10" s="131" t="s">
-        <v>124</v>
-      </c>
-      <c r="K10" s="130"/>
+      <c r="J10" s="113" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" s="112"/>
     </row>
     <row r="11" spans="2:11">
-      <c r="B11" s="41"/>
-      <c r="C11" s="131"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="125"/>
-      <c r="G11" s="125"/>
-      <c r="H11" s="125"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="131"/>
-      <c r="K11" s="130"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="113"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="107"/>
+      <c r="F11" s="107"/>
+      <c r="G11" s="107"/>
+      <c r="H11" s="107"/>
+      <c r="I11" s="111"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="112"/>
     </row>
     <row r="12" spans="2:11">
-      <c r="B12" s="41"/>
-      <c r="C12" s="131"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
-      <c r="F12" s="125"/>
-      <c r="G12" s="125"/>
-      <c r="H12" s="125"/>
-      <c r="I12" s="129"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="113"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="111"/>
       <c r="J12"/>
-      <c r="K12" s="130"/>
+      <c r="K12" s="112"/>
     </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="41"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
-      <c r="F13" s="125"/>
-      <c r="G13" s="125"/>
-      <c r="H13" s="125"/>
-      <c r="I13" s="129"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="107"/>
+      <c r="G13" s="107"/>
+      <c r="H13" s="107"/>
+      <c r="I13" s="111"/>
       <c r="J13"/>
-      <c r="K13" s="130"/>
+      <c r="K13" s="112"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="41"/>
-      <c r="C14" s="131"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="129"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="113"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="111"/>
       <c r="J14"/>
-      <c r="K14" s="130"/>
+      <c r="K14" s="112"/>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="41"/>
-      <c r="C15" s="131"/>
-      <c r="D15" s="125"/>
-      <c r="E15" s="125"/>
-      <c r="F15" s="125"/>
-      <c r="G15" s="125"/>
-      <c r="H15" s="125"/>
-      <c r="I15" s="129"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
+      <c r="F15" s="107"/>
+      <c r="G15" s="107"/>
+      <c r="H15" s="107"/>
+      <c r="I15" s="111"/>
       <c r="J15"/>
-      <c r="K15" s="130"/>
+      <c r="K15" s="112"/>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="41"/>
-      <c r="C16" s="131"/>
-      <c r="D16" s="125"/>
-      <c r="E16" s="125"/>
-      <c r="F16" s="125"/>
-      <c r="G16" s="125"/>
-      <c r="H16" s="125"/>
-      <c r="I16" s="129"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="107"/>
+      <c r="H16" s="107"/>
+      <c r="I16" s="111"/>
       <c r="J16"/>
-      <c r="K16" s="130"/>
+      <c r="K16" s="112"/>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="41"/>
-      <c r="C17" s="131"/>
-      <c r="D17" s="125"/>
-      <c r="E17" s="125"/>
-      <c r="F17" s="125"/>
-      <c r="G17" s="125"/>
-      <c r="H17" s="125"/>
-      <c r="I17" s="129"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
+      <c r="F17" s="107"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
+      <c r="I17" s="111"/>
       <c r="J17"/>
-      <c r="K17" s="130"/>
+      <c r="K17" s="112"/>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="41"/>
-      <c r="C18" s="131"/>
-      <c r="D18" s="125"/>
-      <c r="E18" s="125"/>
-      <c r="F18" s="125"/>
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="129"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="113"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="107"/>
+      <c r="F18" s="107"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="107"/>
+      <c r="I18" s="111"/>
       <c r="J18"/>
-      <c r="K18" s="130"/>
+      <c r="K18" s="112"/>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="41"/>
-      <c r="C19" s="131"/>
-      <c r="D19" s="125"/>
-      <c r="E19" s="125"/>
-      <c r="F19" s="125"/>
-      <c r="G19" s="125"/>
-      <c r="H19" s="125"/>
-      <c r="I19" s="129"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="113"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="111"/>
       <c r="J19"/>
-      <c r="K19" s="130"/>
+      <c r="K19" s="112"/>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="41"/>
-      <c r="C20" s="131"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="125"/>
-      <c r="F20" s="125"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="129"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="113"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="111"/>
       <c r="J20"/>
-      <c r="K20" s="130"/>
+      <c r="K20" s="112"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="41"/>
-      <c r="K21" s="127"/>
+      <c r="B21" s="38"/>
+      <c r="K21" s="109"/>
     </row>
     <row r="22" spans="2:11" ht="17" thickBot="1">
-      <c r="B22" s="132"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
-      <c r="G22" s="133"/>
-      <c r="H22" s="133"/>
-      <c r="I22" s="133"/>
-      <c r="J22" s="134"/>
-      <c r="K22" s="135"/>
+      <c r="B22" s="114"/>
+      <c r="C22" s="115"/>
+      <c r="D22" s="115"/>
+      <c r="E22" s="115"/>
+      <c r="F22" s="115"/>
+      <c r="G22" s="115"/>
+      <c r="H22" s="115"/>
+      <c r="I22" s="115"/>
+      <c r="J22" s="116"/>
+      <c r="K22" s="117"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4348,552 +4353,552 @@
   </sheetPr>
   <dimension ref="B2:N187"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="33.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.33203125" style="36" customWidth="1"/>
-    <col min="2" max="2" width="3.5" style="36" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.33203125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="116" style="37" customWidth="1"/>
-    <col min="11" max="11" width="13.5" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="33.1640625" style="36"/>
+    <col min="1" max="1" width="3.33203125" style="33" customWidth="1"/>
+    <col min="2" max="2" width="3.5" style="33" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="116" style="34" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="33.1640625" style="33"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14" ht="17" thickBot="1"/>
     <row r="3" spans="2:14">
-      <c r="B3" s="38"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="126"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="108"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="124"/>
-      <c r="C4" s="45" t="s">
+      <c r="B4" s="106"/>
+      <c r="C4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="45" t="s">
+      <c r="D4" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="G4" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="F4" s="45" t="s">
+      <c r="H4" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="42" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="45" t="s">
+      <c r="K4" s="110" t="s">
         <v>98</v>
       </c>
-      <c r="H4" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="K4" s="128" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="41"/>
-      <c r="C5" s="36" t="str">
+      <c r="B5" s="38"/>
+      <c r="C5" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>127</v>
-      </c>
-      <c r="F5" s="137">
+      <c r="D5" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="119">
         <v>0.01</v>
       </c>
-      <c r="G5" s="137">
+      <c r="G5" s="119">
         <v>0.04</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="33">
         <f>AVERAGE(F5:G5)</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="J5" s="36"/>
-      <c r="K5" s="127" t="s">
-        <v>102</v>
-      </c>
-      <c r="N5" s="42" t="s">
-        <v>102</v>
+      <c r="I5" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5" s="33"/>
+      <c r="K5" s="109" t="s">
+        <v>100</v>
+      </c>
+      <c r="N5" s="39" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="41"/>
-      <c r="C6" s="36" t="str">
+      <c r="B6" s="38"/>
+      <c r="C6" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D6" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="137">
+      <c r="D6" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="119">
         <v>1500</v>
       </c>
-      <c r="G6" s="137">
+      <c r="G6" s="119">
         <v>2000</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="33">
         <f>AVERAGE(F6:G6)</f>
         <v>1750</v>
       </c>
-      <c r="I6" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>118</v>
-      </c>
-      <c r="K6" s="127" t="s">
-        <v>102</v>
+      <c r="I6" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="J6" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="109" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="41"/>
-      <c r="C7" s="36" t="str">
+      <c r="B7" s="38"/>
+      <c r="C7" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="H7" s="137">
+      <c r="E7" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="H7" s="119">
         <v>30</v>
       </c>
-      <c r="I7" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="36"/>
-      <c r="K7" s="127" t="s">
-        <v>102</v>
+      <c r="I7" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" s="33"/>
+      <c r="K7" s="109" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="41"/>
-      <c r="C8" s="36" t="str">
+      <c r="B8" s="38"/>
+      <c r="C8" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>120</v>
-      </c>
-      <c r="F8" s="36">
+      <c r="E8" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="33">
         <f>(F5*10^9)/(G6*3600)</f>
         <v>1.3888888888888888</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="33">
         <f>(G5*10^9)/(F6*3600)</f>
         <v>7.4074074074074074</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="33">
         <f>AVERAGE(F8:G8)</f>
         <v>4.3981481481481479</v>
       </c>
-      <c r="I8" s="36" t="s">
+      <c r="I8" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="K8" s="127" t="s">
-        <v>102</v>
+      <c r="J8" s="33" t="s">
+        <v>120</v>
+      </c>
+      <c r="K8" s="109" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="41"/>
-      <c r="C9" s="36" t="str">
+      <c r="B9" s="38"/>
+      <c r="C9" s="33" t="str">
         <f>Sources!$E$10</f>
         <v>Kengetallen aquathermie</v>
       </c>
-      <c r="D9" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="E9" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="F9" s="137">
+      <c r="D9" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" s="119">
         <v>2.7</v>
       </c>
-      <c r="G9" s="137">
+      <c r="G9" s="119">
         <v>3.9</v>
       </c>
-      <c r="H9" s="125">
+      <c r="H9" s="107">
         <f>AVERAGE(F9:G9)</f>
         <v>3.3</v>
       </c>
-      <c r="I9" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="J9" s="36" t="s">
-        <v>129</v>
-      </c>
-      <c r="K9" s="127" t="s">
-        <v>108</v>
+      <c r="I9" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="J9" s="33" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" s="109" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="41"/>
-      <c r="C10" s="36" t="str">
+      <c r="B10" s="38"/>
+      <c r="C10" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="33" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="F10" s="119"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="119">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J10" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="F10" s="137"/>
-      <c r="G10" s="137"/>
-      <c r="H10" s="137">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="J10" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="K10" s="127" t="s">
-        <v>102</v>
+      <c r="K10" s="109" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="41"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="125"/>
-      <c r="J11" s="36"/>
-      <c r="K11" s="127"/>
+      <c r="B11" s="38"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
+      <c r="H11" s="107"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="109"/>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="41"/>
-      <c r="C12" s="36" t="str">
+      <c r="B12" s="38"/>
+      <c r="C12" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D12" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" s="138">
+      <c r="D12" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="120">
         <f>166*10^6*$H$5</f>
         <v>4150000</v>
       </c>
-      <c r="G12" s="138">
+      <c r="G12" s="120">
         <f>395*10^6*H5</f>
         <v>9875000</v>
       </c>
-      <c r="H12" s="138">
+      <c r="H12" s="120">
         <f t="shared" ref="H12:H18" si="0">AVERAGE(F12:G12)</f>
         <v>7012500</v>
       </c>
-      <c r="I12" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="J12" s="36" t="s">
-        <v>133</v>
-      </c>
-      <c r="K12" s="127" t="s">
-        <v>102</v>
+      <c r="I12" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J12" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="K12" s="109" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="41"/>
-      <c r="C13" s="36" t="str">
+      <c r="B13" s="38"/>
+      <c r="C13" s="33" t="str">
         <f>Sources!$E$10</f>
         <v>Kengetallen aquathermie</v>
       </c>
-      <c r="D13" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F13" s="138">
+      <c r="D13" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="120">
         <f>1200*$H$8*10^3</f>
         <v>5277777.7777777771</v>
       </c>
-      <c r="G13" s="138">
+      <c r="G13" s="120">
         <f>1300*$H$8*10^3</f>
         <v>5717592.5925925924</v>
       </c>
-      <c r="H13" s="138">
+      <c r="H13" s="120">
         <f t="shared" si="0"/>
         <v>5497685.1851851847</v>
       </c>
-      <c r="I13" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="K13" s="127" t="s">
-        <v>113</v>
+      <c r="I13" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J13" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="K13" s="109" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="2:14" ht="34">
-      <c r="B14" s="41"/>
-      <c r="C14" s="36" t="str">
+      <c r="B14" s="38"/>
+      <c r="C14" s="33" t="str">
         <f>Sources!$E$8</f>
         <v>Functioneel ontwerp 5.0 Vesta MAIS</v>
       </c>
-      <c r="D14" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="F14" s="138">
+      <c r="D14" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F14" s="120">
         <f>90000+198*$H$8*10^3</f>
         <v>960833.33333333326</v>
       </c>
-      <c r="G14" s="138">
+      <c r="G14" s="120">
         <f>110000+242*$H$8*10^3</f>
         <v>1174351.8518518517</v>
       </c>
-      <c r="H14" s="138">
+      <c r="H14" s="120">
         <f t="shared" si="0"/>
         <v>1067592.5925925924</v>
       </c>
-      <c r="I14" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="J14" s="140" t="s">
+      <c r="I14" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J14" s="122" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" s="109" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="34">
+      <c r="B15" s="38"/>
+      <c r="D15" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>143</v>
       </c>
-      <c r="K14" s="127" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" ht="34">
-      <c r="B15" s="41"/>
-      <c r="D15" s="36" t="s">
-        <v>144</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>145</v>
-      </c>
-      <c r="F15" s="138">
+      <c r="F15" s="120">
         <f>135000+103.5*$H$8*10^3</f>
         <v>590208.33333333326</v>
       </c>
-      <c r="G15" s="138">
+      <c r="G15" s="120">
         <f>165000+126.5*$H$8*10^3</f>
         <v>721365.74074074079</v>
       </c>
-      <c r="H15" s="138">
+      <c r="H15" s="120">
         <f t="shared" si="0"/>
         <v>655787.03703703708</v>
       </c>
-      <c r="I15" s="36" t="s">
-        <v>153</v>
-      </c>
-      <c r="J15" s="140" t="s">
-        <v>146</v>
-      </c>
-      <c r="K15" s="127"/>
+      <c r="I15" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="J15" s="122" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="109"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="41"/>
-      <c r="C16" s="36" t="str">
+      <c r="B16" s="38"/>
+      <c r="C16" s="33" t="str">
         <f>Sources!$E$10</f>
         <v>Kengetallen aquathermie</v>
       </c>
-      <c r="D16" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="138">
+      <c r="D16" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F16" s="120">
         <f>26*H8*10^3</f>
         <v>114351.85185185185</v>
       </c>
-      <c r="G16" s="138">
+      <c r="G16" s="120">
         <f>28*H8*10^3</f>
         <v>123148.14814814813</v>
       </c>
-      <c r="H16" s="138">
+      <c r="H16" s="120">
         <f t="shared" si="0"/>
         <v>118750</v>
       </c>
-      <c r="I16" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="J16" s="36" t="s">
-        <v>134</v>
-      </c>
-      <c r="K16" s="127" t="s">
-        <v>114</v>
+      <c r="I16" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J16" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="K16" s="109" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="41"/>
-      <c r="C17" s="36" t="str">
+      <c r="B17" s="38"/>
+      <c r="C17" s="33" t="str">
         <f>Sources!$E$9</f>
         <v>Aquathermal surface water factsheet</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="138">
+      <c r="D17" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="120">
         <f>3*10^6*$H$5</f>
         <v>75000</v>
       </c>
-      <c r="G17" s="138">
+      <c r="G17" s="120">
         <f>8*10^6*$H$5</f>
         <v>200000</v>
       </c>
-      <c r="H17" s="138">
+      <c r="H17" s="120">
         <f t="shared" si="0"/>
         <v>137500</v>
       </c>
-      <c r="I17" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="J17" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="K17" s="127" t="s">
-        <v>102</v>
+      <c r="I17" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J17" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="K17" s="109" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="41"/>
-      <c r="C18" s="36" t="str">
+      <c r="B18" s="38"/>
+      <c r="C18" s="33" t="str">
         <f>Sources!$E$8</f>
         <v>Functioneel ontwerp 5.0 Vesta MAIS</v>
       </c>
-      <c r="D18" s="36" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>132</v>
-      </c>
-      <c r="F18" s="138">
+      <c r="D18" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="120">
         <f>0.01*$H$13</f>
         <v>54976.851851851847</v>
       </c>
-      <c r="G18" s="138">
+      <c r="G18" s="120">
         <f>0.01*H12</f>
         <v>70125</v>
       </c>
-      <c r="H18" s="138">
+      <c r="H18" s="120">
         <f t="shared" si="0"/>
         <v>62550.925925925927</v>
       </c>
-      <c r="I18" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="J18" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="K18" s="127" t="s">
-        <v>115</v>
+      <c r="I18" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="K18" s="109" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="41"/>
-      <c r="C19" s="36" t="str">
+      <c r="B19" s="38"/>
+      <c r="C19" s="33" t="str">
         <f>Sources!$E$8</f>
         <v>Functioneel ontwerp 5.0 Vesta MAIS</v>
       </c>
-      <c r="D19" s="36" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="F19" s="138"/>
-      <c r="G19" s="138"/>
-      <c r="H19" s="138">
+      <c r="D19" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" s="33" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="120"/>
+      <c r="G19" s="120"/>
+      <c r="H19" s="120">
         <f>0.02*H15</f>
         <v>13115.740740740743</v>
       </c>
-      <c r="I19" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="J19" s="36" t="s">
-        <v>137</v>
-      </c>
-      <c r="K19" s="127" t="s">
-        <v>115</v>
+      <c r="I19" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="J19" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="K19" s="109" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="20" spans="2:11" ht="17" thickBot="1">
-      <c r="B20" s="132"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="133"/>
-      <c r="E20" s="133"/>
-      <c r="F20" s="133"/>
-      <c r="G20" s="133"/>
-      <c r="H20" s="133"/>
-      <c r="I20" s="133"/>
-      <c r="J20" s="133"/>
-      <c r="K20" s="135"/>
+      <c r="B20" s="114"/>
+      <c r="C20" s="115"/>
+      <c r="D20" s="115"/>
+      <c r="E20" s="115"/>
+      <c r="F20" s="115"/>
+      <c r="G20" s="115"/>
+      <c r="H20" s="115"/>
+      <c r="I20" s="115"/>
+      <c r="J20" s="115"/>
+      <c r="K20" s="117"/>
     </row>
     <row r="21" spans="2:11">
-      <c r="J21" s="36"/>
+      <c r="J21" s="33"/>
     </row>
     <row r="61" spans="14:14">
-      <c r="N61" s="42" t="s">
-        <v>108</v>
+      <c r="N61" s="39" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="14:14">
-      <c r="N92" s="42" t="s">
+      <c r="N92" s="39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="126" spans="14:14">
+      <c r="N126" s="39" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="158" spans="14:14">
+      <c r="N158" s="39" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="126" spans="14:14">
-      <c r="N126" s="42" t="s">
+    <row r="187" spans="14:14">
+      <c r="N187" s="39" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="158" spans="14:14">
-      <c r="N158" s="42" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="187" spans="14:14">
-      <c r="N187" s="42" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>